<commit_message>
Fuzzy regression, small output file from fuzzy2.py
</commit_message>
<xml_diff>
--- a/Spreadsheets/fuzzyf2.xlsx
+++ b/Spreadsheets/fuzzyf2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BB8D43-9737-417B-BE0C-0830CB14BD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127BE64F-884B-470D-B7D4-BD5EE07D02F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A9055DCF-3041-4AE8-8996-703345412248}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>X</t>
   </si>
@@ -59,15 +59,29 @@
   <si>
     <t>Point ID</t>
   </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>www.MLTechniques.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,10 +116,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -118,8 +133,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -14693,10 +14710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B38634-5279-4D10-B5B6-FDD72934AB44}">
-  <dimension ref="A1:G1001"/>
+  <dimension ref="A1:J1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15072,7 +15089,7 @@
         <v>-15.0720504959229</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>815</v>
       </c>
@@ -15095,7 +15112,7 @@
         <v>77.240878867156297</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>816</v>
       </c>
@@ -15118,7 +15135,7 @@
         <v>-38.228758313364303</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>817</v>
       </c>
@@ -15141,7 +15158,7 @@
         <v>-8.5499441315115607</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>818</v>
       </c>
@@ -15164,7 +15181,7 @@
         <v>33.011531253692901</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>819</v>
       </c>
@@ -15186,8 +15203,14 @@
       <c r="G21" s="2">
         <v>8.5478272169841993</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I21" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>820</v>
       </c>
@@ -15210,7 +15233,7 @@
         <v>23.9837753251634</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>821</v>
       </c>
@@ -15233,7 +15256,7 @@
         <v>-31.452353705105601</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>822</v>
       </c>
@@ -15256,7 +15279,7 @@
         <v>54.726297224226698</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>823</v>
       </c>
@@ -15279,7 +15302,7 @@
         <v>7.9361178453614398</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>824</v>
       </c>
@@ -15302,7 +15325,7 @@
         <v>24.6926389925931</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>825</v>
       </c>
@@ -15325,7 +15348,7 @@
         <v>23.263382322986001</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>826</v>
       </c>
@@ -15348,7 +15371,7 @@
         <v>46.183017399379999</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>827</v>
       </c>
@@ -15371,7 +15394,7 @@
         <v>-19.0378543033098</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>828</v>
       </c>
@@ -15394,7 +15417,7 @@
         <v>22.142473363497601</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>829</v>
       </c>
@@ -15417,7 +15440,7 @@
         <v>-2.6451236205157902</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>830</v>
       </c>
@@ -19928,9 +19951,12 @@
       <c r="E1001" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J21" r:id="rId1" xr:uid="{BA77A4AD-70B4-4F60-84FB-FD3B6A8D4241}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>